<commit_message>
All done with all Example reconciliations.
</commit_message>
<xml_diff>
--- a/CSV-Reconcile_Process/Examples/Results Summary.xlsx
+++ b/CSV-Reconcile_Process/Examples/Results Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/USDA HD/NAL/MyGitFolder/Reconciliation_Project/CSV-Reconcile_Process/Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AC16BC-FB9B-BB4A-93AA-F544CC59F3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7146FF5-D7E1-304B-B0A7-36EAFCEF4D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="5640" windowWidth="31060" windowHeight="12060" xr2:uid="{9F441BA8-D83F-B745-B77C-C4A7D29108DA}"/>
+    <workbookView xWindow="3900" yWindow="2660" windowWidth="27760" windowHeight="15920" xr2:uid="{9F441BA8-D83F-B745-B77C-C4A7D29108DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -77,10 +77,10 @@
     <t>Reconciled</t>
   </si>
   <si>
-    <t>Original # of proposed SME labels (includes duplicates)</t>
-  </si>
-  <si>
-    <t>Original # of proposed SME labels (without duplicates)</t>
+    <t>Proposed SME labels (includes duplicates)</t>
+  </si>
+  <si>
+    <t>Proposed SME labels (without duplicates)</t>
   </si>
 </sst>
 </file>
@@ -594,14 +594,15 @@
   <dimension ref="B4:H11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>

</xml_diff>